<commit_message>
Updated status on 24/2/2021 in video/status_report
</commit_message>
<xml_diff>
--- a/video/status_report/Video_training_status_report.xlsx
+++ b/video/status_report/Video_training_status_report.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t xml:space="preserve">Need to check basic tutorial 2 in gstreamer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/2/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">studied Basic tutorial 2 in gstreamers and 
+ API’s used in basic_tutorial_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to check playback tutorials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/2/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">studied playback turorial-1 and switching 
+between audio streams</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need to add logs to playback tutorial_1 and 
+Check for more info.</t>
   </si>
 </sst>
 </file>
@@ -102,7 +123,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -125,6 +146,12 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -168,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,6 +209,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,10 +233,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -338,6 +369,34 @@
       </c>
       <c r="D10" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="54.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>